<commit_message>
Updated canadensis to canadense
</commit_message>
<xml_diff>
--- a/Table_01_bin_statistics/table/Table_01.xlsx
+++ b/Table_01_bin_statistics/table/Table_01.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\share\manuscripts\02_S2018_L227_111314_metagenomes\08_vs7_revision_01\03_edits\tables_figures\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JTsuji\Downloads\chlorobia-cyc2-genomics\Table_01_bin_statistics\table\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DE9FCD4-6A98-4310-B437-24879F0FC6CE}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{163A6686-B148-4E9E-A851-46155E75293C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="19392" windowHeight="10392" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -99,7 +99,7 @@
         <family val="1"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> canadensis L304-6D</t>
+      <t xml:space="preserve"> canadense L304-6D</t>
     </r>
   </si>
 </sst>
@@ -510,7 +510,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="26.15625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.62890625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.47265625" customWidth="1"/>
     <col min="3" max="3" width="12.05078125" customWidth="1"/>
     <col min="4" max="4" width="8.578125" customWidth="1"/>

</xml_diff>